<commit_message>
Completed preprocessing of facial attractiveness data and extraction of Asian subset
</commit_message>
<xml_diff>
--- a/docs/WBS.xlsx
+++ b/docs/WBS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hataeyeong/Desktop/Study/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hataeyeong/Desktop/Study/LookRank/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124E01EB-6D14-8A41-BE3D-2BB29A59171B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D7C913-0375-5D42-8479-D24FF062345D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3860" yWindow="2220" windowWidth="28100" windowHeight="17380" xr2:uid="{D17D9E39-A022-D543-A913-32A676A19EC4}"/>
+    <workbookView xWindow="3420" yWindow="2220" windowWidth="28540" windowHeight="17380" xr2:uid="{D17D9E39-A022-D543-A913-32A676A19EC4}"/>
   </bookViews>
   <sheets>
     <sheet name="WBS" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="76">
   <si>
     <t>대분류</t>
   </si>
@@ -57,194 +57,231 @@
     <t>2. 데이터 준비 및 수집</t>
   </si>
   <si>
+    <t>외모 점수 산출 기준 및 순위 방식 설계</t>
+  </si>
+  <si>
+    <t>익명화 및 데이터 프라이버시 고려 방안 수립</t>
+  </si>
+  <si>
+    <t>3. AI 모델 개발 및 구현</t>
+  </si>
+  <si>
+    <t>얼굴 인식 관련 라이브러리 설치 및 테스트 (Dlib, FaceNet)</t>
+  </si>
+  <si>
+    <t>얼굴 특징 추출 및 임베딩 알고리즘 구현</t>
+  </si>
+  <si>
+    <t>외모 점수/순위 산출 알고리즘 개발 및 시범 적용</t>
+  </si>
+  <si>
+    <t>TensorFlow 또는 PyTorch 환경 설정 및 모델 학습(필요 시)</t>
+  </si>
+  <si>
+    <t>모델 결과 테스트 및 품질 평가</t>
+  </si>
+  <si>
+    <t>4. 백엔드 개발 (Flask)</t>
+  </si>
+  <si>
+    <t>Flask 기본 서버 환경 구축</t>
+  </si>
+  <si>
+    <t>이미지 업로드 기능 구현 및 서버 내 저장 로직 작성</t>
+  </si>
+  <si>
+    <t>AI 모델 연동 API 개발 (분석 요청 처리, 결과 반환)</t>
+  </si>
+  <si>
+    <t>임시 데이터 저장(메모리 또는 파일 시스템 활용) 구현</t>
+  </si>
+  <si>
+    <t>CORS 설정 및 API 보안 기본 조치 적용</t>
+  </si>
+  <si>
+    <t>5. 프론트엔드 개발 (React)</t>
+  </si>
+  <si>
+    <t>React 프로젝트 초기 세팅</t>
+  </si>
+  <si>
+    <t>이미지 업로드 UI 구현</t>
+  </si>
+  <si>
+    <t>서버 API 연동 (axios 활용)</t>
+  </si>
+  <si>
+    <t>분석 결과 수신 및 시각화 구현 (Chart.js 연동)</t>
+  </si>
+  <si>
+    <t>반응형 UI 적용 (PC/모바일 대응)</t>
+  </si>
+  <si>
+    <t>6. 결과 시각화 및 피드백 기능 개발</t>
+  </si>
+  <si>
+    <t>순위 결과 그래프 설계 및 구현 (Chart.js 활용)</t>
+  </si>
+  <si>
+    <t>사용자 맞춤형 피드백 메시지 작성 및 출력 구현</t>
+  </si>
+  <si>
+    <t>UI/UX 개선 및 사용자 경험 최적화</t>
+  </si>
+  <si>
+    <t>7. 통합 테스트 및 디버깅</t>
+  </si>
+  <si>
+    <t>기능별 단위 테스트 수행 (입력부터 결과 도출까지)</t>
+  </si>
+  <si>
+    <t>전체 플로우 통합 테스트</t>
+  </si>
+  <si>
+    <t>버그 수정 및 UI/UX 최종 다듬기</t>
+  </si>
+  <si>
+    <t>성능 및 보안 점검 (업로드, 데이터 처리 등)</t>
+  </si>
+  <si>
+    <t>8. 배포 및 문서화</t>
+  </si>
+  <si>
+    <t>간단한 배포 환경 구축 (로컬 또는 클라우드)</t>
+  </si>
+  <si>
+    <t>사용자 매뉴얼 및 전시회 설명 자료 작성</t>
+  </si>
+  <si>
+    <t>배포 후 발생하는 문제 모니터링 및 대응 준비</t>
+  </si>
+  <si>
+    <t>주요 기능 목록 작성 (얼굴 인식, 순위 산출, 시각화, 피드백)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>간단한 데이터 흐름 및 시스템 구조 개요 작성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체 개발 일정 간략 수립(자기 일정 관리용)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주차</t>
+  </si>
+  <si>
+    <t>시작일</t>
+  </si>
+  <si>
+    <t>주요 작업 내용</t>
+  </si>
+  <si>
+    <t>1주차</t>
+  </si>
+  <si>
+    <t>프로젝트 기획 및 요구사항 정의</t>
+  </si>
+  <si>
+    <t>2주차</t>
+  </si>
+  <si>
+    <t>데이터 준비 및 수집</t>
+  </si>
+  <si>
+    <t>3주차</t>
+  </si>
+  <si>
+    <t>AI 모델 개발 및 구현 시작</t>
+  </si>
+  <si>
+    <t>4주차</t>
+  </si>
+  <si>
+    <t>AI 모델 개발 마무리 및 테스트</t>
+  </si>
+  <si>
+    <t>5주차</t>
+  </si>
+  <si>
+    <t>백엔드 개발 시작</t>
+  </si>
+  <si>
+    <t>6주차</t>
+  </si>
+  <si>
+    <t>백엔드 개발 완료 및 API 구현</t>
+  </si>
+  <si>
+    <t>7주차</t>
+  </si>
+  <si>
+    <t>프론트엔드 개발 및 결과 시각화 구현</t>
+  </si>
+  <si>
+    <t>8주차</t>
+  </si>
+  <si>
+    <t>통합 테스트, 배포 및 문서화</t>
+  </si>
+  <si>
+    <t>✅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>얼굴 이미지 데이터셋 확보(공개 데이터셋 or 직접 수집)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 프로젝트 기획 및 요구사항 정의</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서비스 목표 및 핵심 기능 정리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>github 초기 세팅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>접수중</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.1.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.1.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SCUT-FBP5500 (외모데이터)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Aihub (한국인 안면 이미지)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>이미지 전처리 코드 작성(OpenCV 활용, 크기 조정 및 정규화)</t>
-  </si>
-  <si>
-    <t>외모 점수 산출 기준 및 순위 방식 설계</t>
-  </si>
-  <si>
-    <t>익명화 및 데이터 프라이버시 고려 방안 수립</t>
-  </si>
-  <si>
-    <t>3. AI 모델 개발 및 구현</t>
-  </si>
-  <si>
-    <t>얼굴 인식 관련 라이브러리 설치 및 테스트 (Dlib, FaceNet)</t>
-  </si>
-  <si>
-    <t>얼굴 특징 추출 및 임베딩 알고리즘 구현</t>
-  </si>
-  <si>
-    <t>외모 점수/순위 산출 알고리즘 개발 및 시범 적용</t>
-  </si>
-  <si>
-    <t>TensorFlow 또는 PyTorch 환경 설정 및 모델 학습(필요 시)</t>
-  </si>
-  <si>
-    <t>모델 결과 테스트 및 품질 평가</t>
-  </si>
-  <si>
-    <t>4. 백엔드 개발 (Flask)</t>
-  </si>
-  <si>
-    <t>Flask 기본 서버 환경 구축</t>
-  </si>
-  <si>
-    <t>이미지 업로드 기능 구현 및 서버 내 저장 로직 작성</t>
-  </si>
-  <si>
-    <t>AI 모델 연동 API 개발 (분석 요청 처리, 결과 반환)</t>
-  </si>
-  <si>
-    <t>임시 데이터 저장(메모리 또는 파일 시스템 활용) 구현</t>
-  </si>
-  <si>
-    <t>CORS 설정 및 API 보안 기본 조치 적용</t>
-  </si>
-  <si>
-    <t>5. 프론트엔드 개발 (React)</t>
-  </si>
-  <si>
-    <t>React 프로젝트 초기 세팅</t>
-  </si>
-  <si>
-    <t>이미지 업로드 UI 구현</t>
-  </si>
-  <si>
-    <t>서버 API 연동 (axios 활용)</t>
-  </si>
-  <si>
-    <t>분석 결과 수신 및 시각화 구현 (Chart.js 연동)</t>
-  </si>
-  <si>
-    <t>반응형 UI 적용 (PC/모바일 대응)</t>
-  </si>
-  <si>
-    <t>6. 결과 시각화 및 피드백 기능 개발</t>
-  </si>
-  <si>
-    <t>순위 결과 그래프 설계 및 구현 (Chart.js 활용)</t>
-  </si>
-  <si>
-    <t>사용자 맞춤형 피드백 메시지 작성 및 출력 구현</t>
-  </si>
-  <si>
-    <t>UI/UX 개선 및 사용자 경험 최적화</t>
-  </si>
-  <si>
-    <t>7. 통합 테스트 및 디버깅</t>
-  </si>
-  <si>
-    <t>기능별 단위 테스트 수행 (입력부터 결과 도출까지)</t>
-  </si>
-  <si>
-    <t>전체 플로우 통합 테스트</t>
-  </si>
-  <si>
-    <t>버그 수정 및 UI/UX 최종 다듬기</t>
-  </si>
-  <si>
-    <t>성능 및 보안 점검 (업로드, 데이터 처리 등)</t>
-  </si>
-  <si>
-    <t>8. 배포 및 문서화</t>
-  </si>
-  <si>
-    <t>간단한 배포 환경 구축 (로컬 또는 클라우드)</t>
-  </si>
-  <si>
-    <t>사용자 매뉴얼 및 전시회 설명 자료 작성</t>
-  </si>
-  <si>
-    <t>배포 후 발생하는 문제 모니터링 및 대응 준비</t>
-  </si>
-  <si>
-    <t>주요 기능 목록 작성 (얼굴 인식, 순위 산출, 시각화, 피드백)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>간단한 데이터 흐름 및 시스템 구조 개요 작성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>전체 개발 일정 간략 수립(자기 일정 관리용)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주차</t>
-  </si>
-  <si>
-    <t>시작일</t>
-  </si>
-  <si>
-    <t>주요 작업 내용</t>
-  </si>
-  <si>
-    <t>1주차</t>
-  </si>
-  <si>
-    <t>프로젝트 기획 및 요구사항 정의</t>
-  </si>
-  <si>
-    <t>2주차</t>
-  </si>
-  <si>
-    <t>데이터 준비 및 수집</t>
-  </si>
-  <si>
-    <t>3주차</t>
-  </si>
-  <si>
-    <t>AI 모델 개발 및 구현 시작</t>
-  </si>
-  <si>
-    <t>4주차</t>
-  </si>
-  <si>
-    <t>AI 모델 개발 마무리 및 테스트</t>
-  </si>
-  <si>
-    <t>5주차</t>
-  </si>
-  <si>
-    <t>백엔드 개발 시작</t>
-  </si>
-  <si>
-    <t>6주차</t>
-  </si>
-  <si>
-    <t>백엔드 개발 완료 및 API 구현</t>
-  </si>
-  <si>
-    <t>7주차</t>
-  </si>
-  <si>
-    <t>프론트엔드 개발 및 결과 시각화 구현</t>
-  </si>
-  <si>
-    <t>8주차</t>
-  </si>
-  <si>
-    <t>통합 테스트, 배포 및 문서화</t>
-  </si>
-  <si>
-    <t>✅</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>얼굴 이미지 데이터셋 확보(공개 데이터셋 or 직접 수집)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. 프로젝트 기획 및 요구사항 정의</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>서비스 목표 및 핵심 기능 정리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>github 초기 세팅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.2.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SCUT-FBP5500 (아시아인 추출)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.2.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OpenCV 활용, 크기 조정 및 정규화</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -252,7 +289,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <numFmts count="1">
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+  </numFmts>
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -292,6 +332,14 @@
       <sz val="16"/>
       <color theme="1"/>
       <name val="Apple Color Emoji"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -363,12 +411,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -405,8 +456,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="쉼표 [0]" xfId="1" builtinId="6"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -739,16 +800,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B641EF4-C72A-B347-875F-D6BD1A93EE6E}">
-  <dimension ref="B2:E51"/>
+  <dimension ref="B2:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="94" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
     <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="61.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -757,7 +818,7 @@
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -769,75 +830,75 @@
     </row>
     <row r="3" spans="2:5" ht="31" customHeight="1">
       <c r="B3" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="13">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="4">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>65</v>
-      </c>
       <c r="E3" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="31" customHeight="1">
       <c r="B4" s="10"/>
-      <c r="C4" s="4">
+      <c r="C4" s="13">
         <v>1.2</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="31" customHeight="1">
       <c r="B5" s="10"/>
-      <c r="C5" s="4">
+      <c r="C5" s="13">
         <v>1.3</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="31" customHeight="1">
       <c r="B6" s="10"/>
-      <c r="C6" s="4">
+      <c r="C6" s="13">
         <v>1.4</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="31" customHeight="1">
       <c r="B7" s="11"/>
-      <c r="C7" s="4">
+      <c r="C7" s="13">
         <v>1.5</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="37" customHeight="1">
       <c r="B8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="13">
         <v>2.1</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>4</v>
@@ -845,61 +906,59 @@
     </row>
     <row r="9" spans="2:5" ht="37" customHeight="1">
       <c r="B9" s="10"/>
-      <c r="C9" s="4">
-        <v>2.2000000000000002</v>
+      <c r="C9" s="13" t="s">
+        <v>67</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>6</v>
+        <v>70</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="37" customHeight="1">
       <c r="B10" s="10"/>
-      <c r="C10" s="4">
-        <v>2.2999999999999998</v>
+      <c r="C10" s="13" t="s">
+        <v>68</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>4</v>
+        <v>69</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="37" customHeight="1">
-      <c r="B11" s="11"/>
-      <c r="C11" s="4">
-        <v>2.4</v>
+      <c r="B11" s="10"/>
+      <c r="C11" s="13">
+        <v>2.2000000000000002</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="37" customHeight="1">
-      <c r="B12" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="4">
-        <v>3.1</v>
+      <c r="B12" s="10"/>
+      <c r="C12" s="13" t="s">
+        <v>72</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>4</v>
+        <v>73</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="37" customHeight="1">
       <c r="B13" s="10"/>
-      <c r="C13" s="4">
-        <v>3.2</v>
+      <c r="C13" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>4</v>
@@ -907,49 +966,49 @@
     </row>
     <row r="14" spans="2:5" ht="37" customHeight="1">
       <c r="B14" s="10"/>
-      <c r="C14" s="4">
-        <v>3.3</v>
+      <c r="C14" s="13">
+        <v>2.2999999999999998</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="37" customHeight="1">
-      <c r="B15" s="10"/>
-      <c r="C15" s="4">
-        <v>3.4</v>
+      <c r="B15" s="11"/>
+      <c r="C15" s="13">
+        <v>2.4</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="37" customHeight="1">
-      <c r="B16" s="11"/>
-      <c r="C16" s="4">
-        <v>3.5</v>
+      <c r="B16" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="13">
+        <v>3.1</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="37" customHeight="1">
-      <c r="B17" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="4">
-        <v>4.0999999999999996</v>
+      <c r="B17" s="10"/>
+      <c r="C17" s="13">
+        <v>3.2</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>4</v>
@@ -957,11 +1016,11 @@
     </row>
     <row r="18" spans="2:5" ht="37" customHeight="1">
       <c r="B18" s="10"/>
-      <c r="C18" s="4">
-        <v>4.2</v>
+      <c r="C18" s="13">
+        <v>3.3</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>4</v>
@@ -969,49 +1028,49 @@
     </row>
     <row r="19" spans="2:5" ht="37" customHeight="1">
       <c r="B19" s="10"/>
-      <c r="C19" s="4">
-        <v>4.3</v>
+      <c r="C19" s="13">
+        <v>3.4</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="37" customHeight="1">
-      <c r="B20" s="10"/>
-      <c r="C20" s="4">
-        <v>4.4000000000000004</v>
+      <c r="B20" s="11"/>
+      <c r="C20" s="13">
+        <v>3.5</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="37" customHeight="1">
-      <c r="B21" s="11"/>
-      <c r="C21" s="4">
-        <v>4.5</v>
+      <c r="B21" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="13">
+        <v>4.0999999999999996</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="37" customHeight="1">
-      <c r="B22" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="4">
-        <v>5.0999999999999996</v>
+      <c r="B22" s="10"/>
+      <c r="C22" s="13">
+        <v>4.2</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>4</v>
@@ -1019,11 +1078,11 @@
     </row>
     <row r="23" spans="2:5" ht="37" customHeight="1">
       <c r="B23" s="10"/>
-      <c r="C23" s="4">
-        <v>5.2</v>
+      <c r="C23" s="13">
+        <v>4.3</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>4</v>
@@ -1031,49 +1090,49 @@
     </row>
     <row r="24" spans="2:5" ht="37" customHeight="1">
       <c r="B24" s="10"/>
-      <c r="C24" s="4">
-        <v>5.3</v>
+      <c r="C24" s="13">
+        <v>4.4000000000000004</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="2:5" ht="37" customHeight="1">
-      <c r="B25" s="10"/>
-      <c r="C25" s="4">
-        <v>5.4</v>
+      <c r="B25" s="11"/>
+      <c r="C25" s="13">
+        <v>4.5</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="37" customHeight="1">
-      <c r="B26" s="11"/>
-      <c r="C26" s="4">
-        <v>5.5</v>
+      <c r="B26" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="13">
+        <v>5.0999999999999996</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="27" spans="2:5" ht="37" customHeight="1">
-      <c r="B27" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="4">
-        <v>6.1</v>
+      <c r="B27" s="10"/>
+      <c r="C27" s="13">
+        <v>5.2</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>4</v>
@@ -1081,49 +1140,49 @@
     </row>
     <row r="28" spans="2:5" ht="37" customHeight="1">
       <c r="B28" s="10"/>
-      <c r="C28" s="4">
-        <v>6.2</v>
+      <c r="C28" s="13">
+        <v>5.3</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="29" spans="2:5" ht="37" customHeight="1">
-      <c r="B29" s="11"/>
-      <c r="C29" s="4">
-        <v>6.3</v>
+      <c r="B29" s="10"/>
+      <c r="C29" s="13">
+        <v>5.4</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="30" spans="2:5" ht="37" customHeight="1">
-      <c r="B30" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C30" s="4">
-        <v>7.1</v>
+      <c r="B30" s="11"/>
+      <c r="C30" s="13">
+        <v>5.5</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="31" spans="2:5" ht="37" customHeight="1">
-      <c r="B31" s="10"/>
-      <c r="C31" s="4">
-        <v>7.2</v>
+      <c r="B31" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="13">
+        <v>6.1</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>4</v>
@@ -1131,11 +1190,11 @@
     </row>
     <row r="32" spans="2:5" ht="37" customHeight="1">
       <c r="B32" s="10"/>
-      <c r="C32" s="4">
-        <v>7.3</v>
+      <c r="C32" s="13">
+        <v>6.2</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>4</v>
@@ -1143,11 +1202,11 @@
     </row>
     <row r="33" spans="2:5" ht="37" customHeight="1">
       <c r="B33" s="11"/>
-      <c r="C33" s="4">
-        <v>7.4</v>
+      <c r="C33" s="13">
+        <v>6.3</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>4</v>
@@ -1155,13 +1214,13 @@
     </row>
     <row r="34" spans="2:5" ht="37" customHeight="1">
       <c r="B34" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="4">
-        <v>8.1</v>
+        <v>30</v>
+      </c>
+      <c r="C34" s="13">
+        <v>7.1</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>4</v>
@@ -1169,83 +1228,133 @@
     </row>
     <row r="35" spans="2:5" ht="37" customHeight="1">
       <c r="B35" s="10"/>
-      <c r="C35" s="4">
+      <c r="C35" s="13">
+        <v>7.2</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="37" customHeight="1">
+      <c r="B36" s="10"/>
+      <c r="C36" s="13">
+        <v>7.3</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="37" customHeight="1">
+      <c r="B37" s="11"/>
+      <c r="C37" s="13">
+        <v>7.4</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="37" customHeight="1">
+      <c r="B38" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38" s="13">
+        <v>8.1</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="37" customHeight="1">
+      <c r="B39" s="10"/>
+      <c r="C39" s="13">
         <v>8.1999999999999993</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D39" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" ht="37" customHeight="1">
+      <c r="B40" s="11"/>
+      <c r="C40" s="13">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="D40" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E35" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" ht="37" customHeight="1">
-      <c r="B36" s="11"/>
-      <c r="C36" s="4">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5">
-      <c r="B37" s="2"/>
-    </row>
-    <row r="38" spans="2:5" ht="21">
-      <c r="B38" s="3"/>
-    </row>
-    <row r="39" spans="2:5" ht="21">
-      <c r="B39" s="3"/>
-    </row>
-    <row r="40" spans="2:5">
-      <c r="B40" s="2"/>
-    </row>
-    <row r="41" spans="2:5" ht="23">
-      <c r="B41" s="1"/>
-    </row>
-    <row r="42" spans="2:5">
-      <c r="B42" s="2"/>
+      <c r="E40" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5">
+      <c r="B41" s="2"/>
+    </row>
+    <row r="42" spans="2:5" ht="21">
+      <c r="B42" s="3"/>
     </row>
     <row r="43" spans="2:5" ht="21">
       <c r="B43" s="3"/>
     </row>
-    <row r="44" spans="2:5" ht="21">
-      <c r="B44" s="3"/>
-    </row>
-    <row r="45" spans="2:5" ht="21">
-      <c r="B45" s="3"/>
+    <row r="44" spans="2:5">
+      <c r="B44" s="2"/>
+    </row>
+    <row r="45" spans="2:5" ht="23">
+      <c r="B45" s="1"/>
     </row>
     <row r="46" spans="2:5">
       <c r="B46" s="2"/>
     </row>
-    <row r="47" spans="2:5" ht="23">
-      <c r="B47" s="1"/>
-    </row>
-    <row r="48" spans="2:5">
-      <c r="B48" s="2"/>
+    <row r="47" spans="2:5" ht="21">
+      <c r="B47" s="3"/>
+    </row>
+    <row r="48" spans="2:5" ht="21">
+      <c r="B48" s="3"/>
     </row>
     <row r="49" spans="2:2" ht="21">
       <c r="B49" s="3"/>
     </row>
-    <row r="50" spans="2:2" ht="21">
-      <c r="B50" s="3"/>
-    </row>
-    <row r="51" spans="2:2" ht="21">
-      <c r="B51" s="3"/>
+    <row r="50" spans="2:2">
+      <c r="B50" s="2"/>
+    </row>
+    <row r="51" spans="2:2" ht="23">
+      <c r="B51" s="1"/>
+    </row>
+    <row r="52" spans="2:2">
+      <c r="B52" s="2"/>
+    </row>
+    <row r="53" spans="2:2" ht="21">
+      <c r="B53" s="3"/>
+    </row>
+    <row r="54" spans="2:2" ht="21">
+      <c r="B54" s="3"/>
+    </row>
+    <row r="55" spans="2:2" ht="21">
+      <c r="B55" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="B38:B40"/>
     <mergeCell ref="B3:B7"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="B17:B21"/>
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="B8:B15"/>
+    <mergeCell ref="B16:B20"/>
+    <mergeCell ref="B21:B25"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="B31:B33"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1269,101 +1378,101 @@
   <sheetData>
     <row r="2" spans="2:4" ht="21">
       <c r="B2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="21">
       <c r="B3" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="7">
         <v>45875</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="21">
       <c r="B4" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="7">
         <v>45882</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="21">
       <c r="B5" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" s="7">
         <v>45889</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="21">
       <c r="B6" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="7">
         <v>45896</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="21">
       <c r="B7" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" s="7">
         <v>45903</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="21">
       <c r="B8" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" s="7">
         <v>45910</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="21">
       <c r="B9" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="7">
         <v>45917</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="21">
       <c r="B10" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C10" s="7">
         <v>45924</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update requirements.txt & Installed and tested face recognition libraries (Dlib, FaceNet)
</commit_message>
<xml_diff>
--- a/docs/WBS.xlsx
+++ b/docs/WBS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hataeyeong/Desktop/Study/LookRank/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D7C913-0375-5D42-8479-D24FF062345D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0441A9F-97BD-BA42-9233-385C0FAF7764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="2220" windowWidth="28540" windowHeight="17380" xr2:uid="{D17D9E39-A022-D543-A913-32A676A19EC4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20340" xr2:uid="{D17D9E39-A022-D543-A913-32A676A19EC4}"/>
   </bookViews>
   <sheets>
     <sheet name="WBS" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="80">
   <si>
     <t>대분류</t>
   </si>
@@ -54,234 +54,253 @@
     <t>[ ]</t>
   </si>
   <si>
+    <t>외모 점수 산출 기준 및 순위 방식 설계</t>
+  </si>
+  <si>
+    <t>익명화 및 데이터 프라이버시 고려 방안 수립</t>
+  </si>
+  <si>
+    <t>얼굴 특징 추출 및 임베딩 알고리즘 구현</t>
+  </si>
+  <si>
+    <t>외모 점수/순위 산출 알고리즘 개발 및 시범 적용</t>
+  </si>
+  <si>
+    <t>TensorFlow 또는 PyTorch 환경 설정 및 모델 학습(필요 시)</t>
+  </si>
+  <si>
+    <t>모델 결과 테스트 및 품질 평가</t>
+  </si>
+  <si>
+    <t>4. 백엔드 개발 (Flask)</t>
+  </si>
+  <si>
+    <t>Flask 기본 서버 환경 구축</t>
+  </si>
+  <si>
+    <t>이미지 업로드 기능 구현 및 서버 내 저장 로직 작성</t>
+  </si>
+  <si>
+    <t>AI 모델 연동 API 개발 (분석 요청 처리, 결과 반환)</t>
+  </si>
+  <si>
+    <t>임시 데이터 저장(메모리 또는 파일 시스템 활용) 구현</t>
+  </si>
+  <si>
+    <t>CORS 설정 및 API 보안 기본 조치 적용</t>
+  </si>
+  <si>
+    <t>5. 프론트엔드 개발 (React)</t>
+  </si>
+  <si>
+    <t>React 프로젝트 초기 세팅</t>
+  </si>
+  <si>
+    <t>이미지 업로드 UI 구현</t>
+  </si>
+  <si>
+    <t>서버 API 연동 (axios 활용)</t>
+  </si>
+  <si>
+    <t>분석 결과 수신 및 시각화 구현 (Chart.js 연동)</t>
+  </si>
+  <si>
+    <t>반응형 UI 적용 (PC/모바일 대응)</t>
+  </si>
+  <si>
+    <t>6. 결과 시각화 및 피드백 기능 개발</t>
+  </si>
+  <si>
+    <t>순위 결과 그래프 설계 및 구현 (Chart.js 활용)</t>
+  </si>
+  <si>
+    <t>사용자 맞춤형 피드백 메시지 작성 및 출력 구현</t>
+  </si>
+  <si>
+    <t>UI/UX 개선 및 사용자 경험 최적화</t>
+  </si>
+  <si>
+    <t>7. 통합 테스트 및 디버깅</t>
+  </si>
+  <si>
+    <t>기능별 단위 테스트 수행 (입력부터 결과 도출까지)</t>
+  </si>
+  <si>
+    <t>전체 플로우 통합 테스트</t>
+  </si>
+  <si>
+    <t>버그 수정 및 UI/UX 최종 다듬기</t>
+  </si>
+  <si>
+    <t>성능 및 보안 점검 (업로드, 데이터 처리 등)</t>
+  </si>
+  <si>
+    <t>8. 배포 및 문서화</t>
+  </si>
+  <si>
+    <t>간단한 배포 환경 구축 (로컬 또는 클라우드)</t>
+  </si>
+  <si>
+    <t>사용자 매뉴얼 및 전시회 설명 자료 작성</t>
+  </si>
+  <si>
+    <t>배포 후 발생하는 문제 모니터링 및 대응 준비</t>
+  </si>
+  <si>
+    <t>주요 기능 목록 작성 (얼굴 인식, 순위 산출, 시각화, 피드백)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>간단한 데이터 흐름 및 시스템 구조 개요 작성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체 개발 일정 간략 수립(자기 일정 관리용)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주차</t>
+  </si>
+  <si>
+    <t>시작일</t>
+  </si>
+  <si>
+    <t>주요 작업 내용</t>
+  </si>
+  <si>
+    <t>1주차</t>
+  </si>
+  <si>
+    <t>프로젝트 기획 및 요구사항 정의</t>
+  </si>
+  <si>
+    <t>2주차</t>
+  </si>
+  <si>
+    <t>데이터 준비 및 수집</t>
+  </si>
+  <si>
+    <t>3주차</t>
+  </si>
+  <si>
+    <t>AI 모델 개발 및 구현 시작</t>
+  </si>
+  <si>
+    <t>4주차</t>
+  </si>
+  <si>
+    <t>AI 모델 개발 마무리 및 테스트</t>
+  </si>
+  <si>
+    <t>5주차</t>
+  </si>
+  <si>
+    <t>백엔드 개발 시작</t>
+  </si>
+  <si>
+    <t>6주차</t>
+  </si>
+  <si>
+    <t>백엔드 개발 완료 및 API 구현</t>
+  </si>
+  <si>
+    <t>7주차</t>
+  </si>
+  <si>
+    <t>프론트엔드 개발 및 결과 시각화 구현</t>
+  </si>
+  <si>
+    <t>8주차</t>
+  </si>
+  <si>
+    <t>통합 테스트, 배포 및 문서화</t>
+  </si>
+  <si>
+    <t>✅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>얼굴 이미지 데이터셋 확보(공개 데이터셋 or 직접 수집)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 프로젝트 기획 및 요구사항 정의</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서비스 목표 및 핵심 기능 정리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>github 초기 세팅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>접수중</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.1.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.1.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SCUT-FBP5500 (외모데이터)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Aihub (한국인 안면 이미지)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이미지 전처리 코드 작성(OpenCV 활용, 크기 조정 및 정규화)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.2.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SCUT-FBP5500 (아시아인 추출)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.2.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OpenCV 활용, 크기 조정 및 정규화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>2. 데이터 준비 및 수집</t>
-  </si>
-  <si>
-    <t>외모 점수 산출 기준 및 순위 방식 설계</t>
-  </si>
-  <si>
-    <t>익명화 및 데이터 프라이버시 고려 방안 수립</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데이터셋 분할(훈련, 검증, 테스트)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>3. AI 모델 개발 및 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>얼굴 인식 관련 라이브러리 설치 및 테스트 (Dlib, FaceNet)</t>
-  </si>
-  <si>
-    <t>얼굴 특징 추출 및 임베딩 알고리즘 구현</t>
-  </si>
-  <si>
-    <t>외모 점수/순위 산출 알고리즘 개발 및 시범 적용</t>
-  </si>
-  <si>
-    <t>TensorFlow 또는 PyTorch 환경 설정 및 모델 학습(필요 시)</t>
-  </si>
-  <si>
-    <t>모델 결과 테스트 및 품질 평가</t>
-  </si>
-  <si>
-    <t>4. 백엔드 개발 (Flask)</t>
-  </si>
-  <si>
-    <t>Flask 기본 서버 환경 구축</t>
-  </si>
-  <si>
-    <t>이미지 업로드 기능 구현 및 서버 내 저장 로직 작성</t>
-  </si>
-  <si>
-    <t>AI 모델 연동 API 개발 (분석 요청 처리, 결과 반환)</t>
-  </si>
-  <si>
-    <t>임시 데이터 저장(메모리 또는 파일 시스템 활용) 구현</t>
-  </si>
-  <si>
-    <t>CORS 설정 및 API 보안 기본 조치 적용</t>
-  </si>
-  <si>
-    <t>5. 프론트엔드 개발 (React)</t>
-  </si>
-  <si>
-    <t>React 프로젝트 초기 세팅</t>
-  </si>
-  <si>
-    <t>이미지 업로드 UI 구현</t>
-  </si>
-  <si>
-    <t>서버 API 연동 (axios 활용)</t>
-  </si>
-  <si>
-    <t>분석 결과 수신 및 시각화 구현 (Chart.js 연동)</t>
-  </si>
-  <si>
-    <t>반응형 UI 적용 (PC/모바일 대응)</t>
-  </si>
-  <si>
-    <t>6. 결과 시각화 및 피드백 기능 개발</t>
-  </si>
-  <si>
-    <t>순위 결과 그래프 설계 및 구현 (Chart.js 활용)</t>
-  </si>
-  <si>
-    <t>사용자 맞춤형 피드백 메시지 작성 및 출력 구현</t>
-  </si>
-  <si>
-    <t>UI/UX 개선 및 사용자 경험 최적화</t>
-  </si>
-  <si>
-    <t>7. 통합 테스트 및 디버깅</t>
-  </si>
-  <si>
-    <t>기능별 단위 테스트 수행 (입력부터 결과 도출까지)</t>
-  </si>
-  <si>
-    <t>전체 플로우 통합 테스트</t>
-  </si>
-  <si>
-    <t>버그 수정 및 UI/UX 최종 다듬기</t>
-  </si>
-  <si>
-    <t>성능 및 보안 점검 (업로드, 데이터 처리 등)</t>
-  </si>
-  <si>
-    <t>8. 배포 및 문서화</t>
-  </si>
-  <si>
-    <t>간단한 배포 환경 구축 (로컬 또는 클라우드)</t>
-  </si>
-  <si>
-    <t>사용자 매뉴얼 및 전시회 설명 자료 작성</t>
-  </si>
-  <si>
-    <t>배포 후 발생하는 문제 모니터링 및 대응 준비</t>
-  </si>
-  <si>
-    <t>주요 기능 목록 작성 (얼굴 인식, 순위 산출, 시각화, 피드백)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>간단한 데이터 흐름 및 시스템 구조 개요 작성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>전체 개발 일정 간략 수립(자기 일정 관리용)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주차</t>
-  </si>
-  <si>
-    <t>시작일</t>
-  </si>
-  <si>
-    <t>주요 작업 내용</t>
-  </si>
-  <si>
-    <t>1주차</t>
-  </si>
-  <si>
-    <t>프로젝트 기획 및 요구사항 정의</t>
-  </si>
-  <si>
-    <t>2주차</t>
-  </si>
-  <si>
-    <t>데이터 준비 및 수집</t>
-  </si>
-  <si>
-    <t>3주차</t>
-  </si>
-  <si>
-    <t>AI 모델 개발 및 구현 시작</t>
-  </si>
-  <si>
-    <t>4주차</t>
-  </si>
-  <si>
-    <t>AI 모델 개발 마무리 및 테스트</t>
-  </si>
-  <si>
-    <t>5주차</t>
-  </si>
-  <si>
-    <t>백엔드 개발 시작</t>
-  </si>
-  <si>
-    <t>6주차</t>
-  </si>
-  <si>
-    <t>백엔드 개발 완료 및 API 구현</t>
-  </si>
-  <si>
-    <t>7주차</t>
-  </si>
-  <si>
-    <t>프론트엔드 개발 및 결과 시각화 구현</t>
-  </si>
-  <si>
-    <t>8주차</t>
-  </si>
-  <si>
-    <t>통합 테스트, 배포 및 문서화</t>
-  </si>
-  <si>
-    <t>✅</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>얼굴 이미지 데이터셋 확보(공개 데이터셋 or 직접 수집)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. 프로젝트 기획 및 요구사항 정의</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>서비스 목표 및 핵심 기능 정리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>github 초기 세팅</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>접수중</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.1.1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.1.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SCUT-FBP5500 (외모데이터)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Aihub (한국인 안면 이미지)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이미지 전처리 코드 작성(OpenCV 활용, 크기 조정 및 정규화)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.2.1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SCUT-FBP5500 (아시아인 추출)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.2.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OpenCV 활용, 크기 조정 및 정규화</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -800,10 +819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B641EF4-C72A-B347-875F-D6BD1A93EE6E}">
-  <dimension ref="B2:E55"/>
+  <dimension ref="B2:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="94" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="94" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -830,16 +849,16 @@
     </row>
     <row r="3" spans="2:5" ht="31" customHeight="1">
       <c r="B3" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C3" s="13">
         <v>1.1000000000000001</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="31" customHeight="1">
@@ -848,10 +867,10 @@
         <v>1.2</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="31" customHeight="1">
@@ -860,10 +879,10 @@
         <v>1.3</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="31" customHeight="1">
@@ -872,10 +891,10 @@
         <v>1.4</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="31" customHeight="1">
@@ -884,21 +903,21 @@
         <v>1.5</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="37" customHeight="1">
       <c r="B8" s="9" t="s">
-        <v>5</v>
+        <v>73</v>
       </c>
       <c r="C8" s="13">
         <v>2.1</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>4</v>
@@ -907,25 +926,25 @@
     <row r="9" spans="2:5" ht="37" customHeight="1">
       <c r="B9" s="10"/>
       <c r="C9" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>70</v>
-      </c>
       <c r="E9" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="37" customHeight="1">
       <c r="B10" s="10"/>
       <c r="C10" s="13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="37" customHeight="1">
@@ -934,93 +953,93 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>4</v>
+        <v>68</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="37" customHeight="1">
       <c r="B12" s="10"/>
       <c r="C12" s="13" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="37" customHeight="1">
       <c r="B13" s="10"/>
       <c r="C13" s="13" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>4</v>
+        <v>72</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="37" customHeight="1">
       <c r="B14" s="10"/>
-      <c r="C14" s="13">
-        <v>2.2999999999999998</v>
+      <c r="C14" s="13" t="s">
+        <v>75</v>
       </c>
       <c r="D14" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="37" customHeight="1">
+      <c r="B15" s="10"/>
+      <c r="C15" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="37" customHeight="1">
+      <c r="B16" s="11"/>
+      <c r="C16" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" ht="37" customHeight="1">
-      <c r="B15" s="11"/>
-      <c r="C15" s="13">
-        <v>2.4</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" ht="37" customHeight="1">
-      <c r="B16" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="13">
+      <c r="E16" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="37" customHeight="1">
+      <c r="B17" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="13">
         <v>3.1</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="37" customHeight="1">
-      <c r="B17" s="10"/>
-      <c r="C17" s="13">
-        <v>3.2</v>
-      </c>
       <c r="D17" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>4</v>
+        <v>79</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="37" customHeight="1">
       <c r="B18" s="10"/>
       <c r="C18" s="13">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>4</v>
@@ -1029,48 +1048,48 @@
     <row r="19" spans="2:5" ht="37" customHeight="1">
       <c r="B19" s="10"/>
       <c r="C19" s="13">
+        <v>3.3</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="37" customHeight="1">
+      <c r="B20" s="10"/>
+      <c r="C20" s="13">
         <v>3.4</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="37" customHeight="1">
+      <c r="B21" s="11"/>
+      <c r="C21" s="13">
+        <v>3.5</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="37" customHeight="1">
+      <c r="B22" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="13">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" ht="37" customHeight="1">
-      <c r="B20" s="11"/>
-      <c r="C20" s="13">
-        <v>3.5</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" ht="37" customHeight="1">
-      <c r="B21" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="13">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" ht="37" customHeight="1">
-      <c r="B22" s="10"/>
-      <c r="C22" s="13">
-        <v>4.2</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>4</v>
@@ -1079,10 +1098,10 @@
     <row r="23" spans="2:5" ht="37" customHeight="1">
       <c r="B23" s="10"/>
       <c r="C23" s="13">
-        <v>4.3</v>
+        <v>4.2</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>4</v>
@@ -1091,48 +1110,48 @@
     <row r="24" spans="2:5" ht="37" customHeight="1">
       <c r="B24" s="10"/>
       <c r="C24" s="13">
+        <v>4.3</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="37" customHeight="1">
+      <c r="B25" s="10"/>
+      <c r="C25" s="13">
         <v>4.4000000000000004</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="37" customHeight="1">
+      <c r="B26" s="11"/>
+      <c r="C26" s="13">
+        <v>4.5</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="37" customHeight="1">
+      <c r="B27" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="13">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="37" customHeight="1">
-      <c r="B25" s="11"/>
-      <c r="C25" s="13">
-        <v>4.5</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" ht="37" customHeight="1">
-      <c r="B26" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" s="13">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" ht="37" customHeight="1">
-      <c r="B27" s="10"/>
-      <c r="C27" s="13">
-        <v>5.2</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>4</v>
@@ -1141,10 +1160,10 @@
     <row r="28" spans="2:5" ht="37" customHeight="1">
       <c r="B28" s="10"/>
       <c r="C28" s="13">
-        <v>5.3</v>
+        <v>5.2</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>4</v>
@@ -1153,86 +1172,86 @@
     <row r="29" spans="2:5" ht="37" customHeight="1">
       <c r="B29" s="10"/>
       <c r="C29" s="13">
+        <v>5.3</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="37" customHeight="1">
+      <c r="B30" s="10"/>
+      <c r="C30" s="13">
         <v>5.4</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D30" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" ht="37" customHeight="1">
+      <c r="B31" s="11"/>
+      <c r="C31" s="13">
+        <v>5.5</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" ht="37" customHeight="1">
+      <c r="B32" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="13">
+        <v>6.1</v>
+      </c>
+      <c r="D32" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E29" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" ht="37" customHeight="1">
-      <c r="B30" s="11"/>
-      <c r="C30" s="13">
-        <v>5.5</v>
-      </c>
-      <c r="D30" s="4" t="s">
+      <c r="E32" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="37" customHeight="1">
+      <c r="B33" s="10"/>
+      <c r="C33" s="13">
+        <v>6.2</v>
+      </c>
+      <c r="D33" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E30" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" ht="37" customHeight="1">
-      <c r="B31" s="9" t="s">
+      <c r="E33" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="37" customHeight="1">
+      <c r="B34" s="11"/>
+      <c r="C34" s="13">
+        <v>6.3</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="13">
-        <v>6.1</v>
-      </c>
-      <c r="D31" s="4" t="s">
+      <c r="E34" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" ht="37" customHeight="1">
+      <c r="B35" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E31" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" ht="37" customHeight="1">
-      <c r="B32" s="10"/>
-      <c r="C32" s="13">
-        <v>6.2</v>
-      </c>
-      <c r="D32" s="4" t="s">
+      <c r="C35" s="13">
+        <v>7.1</v>
+      </c>
+      <c r="D35" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" ht="37" customHeight="1">
-      <c r="B33" s="11"/>
-      <c r="C33" s="13">
-        <v>6.3</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" ht="37" customHeight="1">
-      <c r="B34" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34" s="13">
-        <v>7.1</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" ht="37" customHeight="1">
-      <c r="B35" s="10"/>
-      <c r="C35" s="13">
-        <v>7.2</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>4</v>
@@ -1241,85 +1260,94 @@
     <row r="36" spans="2:5" ht="37" customHeight="1">
       <c r="B36" s="10"/>
       <c r="C36" s="13">
+        <v>7.2</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="37" customHeight="1">
+      <c r="B37" s="10"/>
+      <c r="C37" s="13">
         <v>7.3</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D37" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="37" customHeight="1">
+      <c r="B38" s="11"/>
+      <c r="C38" s="13">
+        <v>7.4</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="37" customHeight="1">
+      <c r="B39" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" s="13">
+        <v>8.1</v>
+      </c>
+      <c r="D39" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E36" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" ht="37" customHeight="1">
-      <c r="B37" s="11"/>
-      <c r="C37" s="13">
-        <v>7.4</v>
-      </c>
-      <c r="D37" s="4" t="s">
+      <c r="E39" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" ht="37" customHeight="1">
+      <c r="B40" s="10"/>
+      <c r="C40" s="13">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D40" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E37" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" ht="37" customHeight="1">
-      <c r="B38" s="9" t="s">
+      <c r="E40" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" ht="37" customHeight="1">
+      <c r="B41" s="11"/>
+      <c r="C41" s="13">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="D41" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C38" s="13">
-        <v>8.1</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" ht="37" customHeight="1">
-      <c r="B39" s="10"/>
-      <c r="C39" s="13">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" ht="37" customHeight="1">
-      <c r="B40" s="11"/>
-      <c r="C40" s="13">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5">
-      <c r="B41" s="2"/>
-    </row>
-    <row r="42" spans="2:5" ht="21">
-      <c r="B42" s="3"/>
+      <c r="E41" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5">
+      <c r="B42" s="2"/>
     </row>
     <row r="43" spans="2:5" ht="21">
       <c r="B43" s="3"/>
     </row>
-    <row r="44" spans="2:5">
-      <c r="B44" s="2"/>
-    </row>
-    <row r="45" spans="2:5" ht="23">
-      <c r="B45" s="1"/>
-    </row>
-    <row r="46" spans="2:5">
-      <c r="B46" s="2"/>
-    </row>
-    <row r="47" spans="2:5" ht="21">
-      <c r="B47" s="3"/>
+    <row r="44" spans="2:5" ht="21">
+      <c r="B44" s="3"/>
+    </row>
+    <row r="45" spans="2:5">
+      <c r="B45" s="2"/>
+    </row>
+    <row r="46" spans="2:5" ht="23">
+      <c r="B46" s="1"/>
+    </row>
+    <row r="47" spans="2:5">
+      <c r="B47" s="2"/>
     </row>
     <row r="48" spans="2:5" ht="21">
       <c r="B48" s="3"/>
@@ -1327,17 +1355,17 @@
     <row r="49" spans="2:2" ht="21">
       <c r="B49" s="3"/>
     </row>
-    <row r="50" spans="2:2">
-      <c r="B50" s="2"/>
-    </row>
-    <row r="51" spans="2:2" ht="23">
-      <c r="B51" s="1"/>
-    </row>
-    <row r="52" spans="2:2">
-      <c r="B52" s="2"/>
-    </row>
-    <row r="53" spans="2:2" ht="21">
-      <c r="B53" s="3"/>
+    <row r="50" spans="2:2" ht="21">
+      <c r="B50" s="3"/>
+    </row>
+    <row r="51" spans="2:2">
+      <c r="B51" s="2"/>
+    </row>
+    <row r="52" spans="2:2" ht="23">
+      <c r="B52" s="1"/>
+    </row>
+    <row r="53" spans="2:2">
+      <c r="B53" s="2"/>
     </row>
     <row r="54" spans="2:2" ht="21">
       <c r="B54" s="3"/>
@@ -1345,16 +1373,19 @@
     <row r="55" spans="2:2" ht="21">
       <c r="B55" s="3"/>
     </row>
+    <row r="56" spans="2:2" ht="21">
+      <c r="B56" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="B39:B41"/>
     <mergeCell ref="B3:B7"/>
-    <mergeCell ref="B8:B15"/>
-    <mergeCell ref="B16:B20"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="B26:B30"/>
-    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="B8:B16"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="B22:B26"/>
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="B32:B34"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1366,7 +1397,7 @@
   <dimension ref="B2:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1378,101 +1409,101 @@
   <sheetData>
     <row r="2" spans="2:4" ht="21">
       <c r="B2" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="21">
       <c r="B3" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C3" s="7">
         <v>45875</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="21">
       <c r="B4" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C4" s="7">
         <v>45882</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="21">
       <c r="B5" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C5" s="7">
         <v>45889</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="21">
       <c r="B6" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C6" s="7">
         <v>45896</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="21">
       <c r="B7" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C7" s="7">
         <v>45903</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="21">
       <c r="B8" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C8" s="7">
         <v>45910</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="21">
       <c r="B9" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C9" s="7">
         <v>45917</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="21">
       <c r="B10" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C10" s="7">
         <v>45924</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>